<commit_message>
added heart sensor & hub
</commit_message>
<xml_diff>
--- a/Compos.xlsx
+++ b/Compos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujux\Documents\GitHub\JWatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D309B-4AFF-4433-97BC-FD4D17B62525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544AEF43-0012-44A1-903E-5ADD05DCD849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{075F82BD-02A2-4454-8243-348703E68BB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{075F82BD-02A2-4454-8243-348703E68BB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Compos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
   <si>
     <t>Composant</t>
   </si>
@@ -50,9 +50,6 @@
     <t>µC</t>
   </si>
   <si>
-    <t>ESP32-S3-MINI-1</t>
-  </si>
-  <si>
     <t>Pin</t>
   </si>
   <si>
@@ -360,6 +357,12 @@
   </si>
   <si>
     <t>HEX</t>
+  </si>
+  <si>
+    <t>lsm6dso</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1-N8R8</t>
   </si>
 </sst>
 </file>
@@ -741,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CCAD86-64C2-4EC0-B9BA-AB0655B9C524}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,44 +767,47 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
         <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -821,192 +827,192 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1030,47 +1036,47 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
       </c>
       <c r="C3" s="2">
         <v>1110110</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,52 +1084,52 @@
         <v>1110111</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
       </c>
       <c r="C5" s="2">
         <v>1011100</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2">
         <v>1101010</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,10 +1137,10 @@
         <v>1101011</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1146,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CB18EB-FCCE-48E9-9C67-959C0750CAA6}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1158,133 +1164,133 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>5.5</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>3.3</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>1.1000000000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <f>60*10^-9</f>
         <v>6.0000000000000008E-8</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <f>45*10^-9</f>
         <v>4.5000000000000006E-8</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
       </c>
       <c r="C7">
         <v>0.22</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <v>0.34</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <f>100*10^-9</f>
         <v>1.0000000000000001E-7</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
         <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,7 +1303,7 @@
         <v>2557499.9999999995</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,7 +1316,7 @@
         <v>710.41666666666652</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,96 +1329,96 @@
         <v>29.600694444444439</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <f>50*10^-3</f>
         <v>0.05</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
         <v>71</v>
-      </c>
-      <c r="B17" t="s">
-        <v>72</v>
       </c>
       <c r="C17">
         <v>1000</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
         <v>75</v>
-      </c>
-      <c r="B18" t="s">
-        <v>76</v>
       </c>
       <c r="C18">
         <f>C3-C8</f>
         <v>2.96</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
         <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>78</v>
       </c>
       <c r="C19">
         <f>C17*C7</f>
         <v>220</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
         <v>79</v>
-      </c>
-      <c r="B20" t="s">
-        <v>80</v>
       </c>
       <c r="C20">
         <f>5*C19</f>
         <v>1100</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21">
         <f>C18/C17</f>
         <v>2.96E-3</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>